<commit_message>
feat(import): importing the data dictionaries
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated_measures.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated_measures.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ProjectGroups\LifeCycle\Pilot\datashield\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E355482-F896-5149-B930-B2A962095B05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>table</t>
   </si>
@@ -37,9 +38,6 @@
     <t>label:en</t>
   </si>
   <si>
-    <t>alias</t>
-  </si>
-  <si>
     <t>child_id</t>
   </si>
   <si>
@@ -200,12 +198,15 @@
   </si>
   <si>
     <t>1_0_monthly_repeated_measures</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,8 +284,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -742,43 +743,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BI14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BG14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E1"/>
+      <c r="F1"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -832,26 +827,22 @@
       <c r="BE1"/>
       <c r="BF1"/>
       <c r="BG1"/>
-      <c r="BH1"/>
-      <c r="BI1"/>
-    </row>
-    <row r="2" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -905,12 +896,10 @@
       <c r="BE2"/>
       <c r="BF2"/>
       <c r="BG2"/>
-      <c r="BH2"/>
-      <c r="BI2"/>
-    </row>
-    <row r="3" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>59</v>
+    </row>
+    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
@@ -921,216 +910,168 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>59</v>
+      <c r="E3"/>
+    </row>
+    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4"/>
+    </row>
+    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4"/>
-    </row>
-    <row r="5" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5"/>
+    </row>
+    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5"/>
-    </row>
-    <row r="6" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6"/>
-    </row>
-    <row r="7" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="E6"/>
+    </row>
+    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7"/>
-    </row>
-    <row r="8" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>59</v>
+        <v>10</v>
+      </c>
+      <c r="E7"/>
+    </row>
+    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8"/>
-    </row>
-    <row r="9" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>48</v>
+      </c>
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9"/>
-    </row>
-    <row r="10" spans="1:61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11"/>
+    </row>
+    <row r="12" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="5" t="s">
+    </row>
+    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="B14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
@@ -1142,32 +1083,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="25.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -1175,12 +1116,12 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4">
         <v>101</v>
@@ -1189,17 +1130,17 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4">
         <v>102</v>
@@ -1208,17 +1149,17 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4">
         <v>103</v>
@@ -1227,17 +1168,17 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4">
         <v>104</v>
@@ -1246,17 +1187,17 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4">
         <v>105</v>
@@ -1265,17 +1206,17 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4">
         <v>106</v>
@@ -1284,17 +1225,17 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4">
         <v>107</v>
@@ -1303,17 +1244,17 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4">
         <v>108</v>
@@ -1322,17 +1263,17 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4">
         <v>109</v>
@@ -1341,17 +1282,17 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4">
         <v>110</v>
@@ -1360,17 +1301,17 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="4">
         <v>111</v>
@@ -1379,17 +1320,17 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4">
         <v>112</v>
@@ -1398,17 +1339,17 @@
         <v>0</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="4">
         <v>113</v>
@@ -1417,17 +1358,17 @@
         <v>0</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="4">
         <v>114</v>
@@ -1436,17 +1377,17 @@
         <v>0</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="4">
         <v>115</v>
@@ -1455,17 +1396,17 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="4">
         <v>116</v>
@@ -1474,17 +1415,17 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="4">
         <v>117</v>
@@ -1493,17 +1434,17 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="4">
         <v>118</v>
@@ -1512,17 +1453,17 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="4">
         <v>119</v>
@@ -1531,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>

</xml_diff>

<commit_message>
chore(packages): added additional packages
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated_measures.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated_measures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E355482-F896-5149-B930-B2A962095B05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0074B65-5D2C-5149-96FE-782D7AFF8AB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
   <si>
     <t>table</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>1_0_monthly_repeated_measures</t>
-  </si>
-  <si>
-    <t>label</t>
   </si>
 </sst>
 </file>
@@ -747,7 +744,7 @@
   <dimension ref="A1:BG14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -770,7 +767,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>

</xml_diff>

<commit_message>
fix(vars): updated vars and data dictionarie
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated_measures.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated_measures.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0074B65-5D2C-5149-96FE-782D7AFF8AB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DC1593-1F7B-C541-B664-E7982E6C1546}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>table</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>1_0_monthly_repeated_measures</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
@@ -767,7 +770,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>

</xml_diff>

<commit_message>
feat(categories): added categories to upload
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated_measures.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated_measures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DC1593-1F7B-C541-B664-E7982E6C1546}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A627D87E-AB21-DB4F-ADAF-70273D15D5BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
-  <si>
-    <t>table</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -35,9 +32,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>label:en</t>
-  </si>
-  <si>
     <t>child_id</t>
   </si>
   <si>
@@ -47,15 +41,9 @@
     <t>numeric</t>
   </si>
   <si>
-    <t>child id</t>
-  </si>
-  <si>
     <t>cohort_id</t>
   </si>
   <si>
-    <t>cohort id</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
@@ -128,15 +116,9 @@
     <t>row_id</t>
   </si>
   <si>
-    <t>row id</t>
-  </si>
-  <si>
     <t>age_months</t>
   </si>
   <si>
-    <t>age of child in months</t>
-  </si>
-  <si>
     <t>height_</t>
   </si>
   <si>
@@ -149,30 +131,12 @@
     <t>weight_age</t>
   </si>
   <si>
-    <t xml:space="preserve">height </t>
-  </si>
-  <si>
-    <t>age at height measurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight </t>
-  </si>
-  <si>
-    <t>age at weight measurement</t>
-  </si>
-  <si>
     <t>age_years</t>
   </si>
   <si>
     <t>coh_country</t>
   </si>
   <si>
-    <t>country id</t>
-  </si>
-  <si>
-    <t>age of child in years</t>
-  </si>
-  <si>
     <t>RUG1</t>
   </si>
   <si>
@@ -182,9 +146,6 @@
     <t>mother_id</t>
   </si>
   <si>
-    <t>mother id</t>
-  </si>
-  <si>
     <t>preg_no</t>
   </si>
   <si>
@@ -197,10 +158,40 @@
     <t>Within-pregnancy birth order</t>
   </si>
   <si>
-    <t>1_0_monthly_repeated_measures</t>
-  </si>
-  <si>
     <t>label</t>
+  </si>
+  <si>
+    <t>Unique identifier for the row</t>
+  </si>
+  <si>
+    <t>Unique identifier for the child</t>
+  </si>
+  <si>
+    <t>Unique identifier for the mother</t>
+  </si>
+  <si>
+    <t>Unique identifier for the cohort</t>
+  </si>
+  <si>
+    <t>Unique identifier for the country</t>
+  </si>
+  <si>
+    <t>Age of child in years</t>
+  </si>
+  <si>
+    <t>Age of child in months</t>
+  </si>
+  <si>
+    <t>Height of the child</t>
+  </si>
+  <si>
+    <t>Age of the child at height measurement</t>
+  </si>
+  <si>
+    <t>Weight of the child</t>
+  </si>
+  <si>
+    <t>Age of the child at weight measurement</t>
   </si>
 </sst>
 </file>
@@ -271,11 +262,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -746,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -760,17 +750,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -829,17 +819,17 @@
       <c r="BG1"/>
     </row>
     <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>34</v>
+      <c r="A2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -899,178 +889,178 @@
     </row>
     <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E8"/>
     </row>
     <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E9"/>
     </row>
     <row r="10" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>42</v>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E11"/>
     </row>
     <row r="12" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>43</v>
+      <c r="A12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>44</v>
+      <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>45</v>
+      <c r="A14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1084,398 +1074,297 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="12.83203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>101</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>102</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>103</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>104</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4">
-        <v>101</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>105</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4">
-        <v>102</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>106</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4">
-        <v>103</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>107</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4">
-        <v>104</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>108</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4">
-        <v>105</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3">
+        <v>109</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="4">
-        <v>106</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3">
+        <v>110</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4">
-        <v>107</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3">
+        <v>111</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4">
-        <v>108</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <v>112</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4">
-        <v>109</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>113</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4">
-        <v>110</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3">
+        <v>114</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="4">
-        <v>111</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3">
+        <v>115</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="4">
-        <v>112</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3">
+        <v>116</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="4">
-        <v>113</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3">
+        <v>117</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="4">
-        <v>114</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="4">
-        <v>115</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="4">
-        <v>116</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="4">
-        <v>117</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="4">
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3">
         <v>118</v>
       </c>
-      <c r="D19" s="6">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3">
         <v>119</v>
       </c>
-      <c r="D20" s="6">
-        <v>0</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>